<commit_message>
add results for H1
</commit_message>
<xml_diff>
--- a/report_sheets/EEGManyPipelines_results_h1.xlsx
+++ b/report_sheets/EEGManyPipelines_results_h1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t xml:space="preserve">Team identifier:</t>
   </si>
@@ -53,6 +53,30 @@
   </si>
   <si>
     <t xml:space="preserve">Interpretation (significant or not)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comment (see our Report.txt file: https://github.com/NomisCiri/eeg_manypipes_arc/blob/main/REPORT.txt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-100 to 200ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fp1, Fpz, Fp2, AF7, AF3, AFz, AF4, AF8, F7, F5, F3, F1, Fz, F2, F4, F6, F8, FC5, FC3, FC1, FCz, FC2, FC4, FC6, C5, C3, C1, Cz, C2, C4, C6, CP3, CP1, CPz, CP2, CP4, P1, Pz, P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cluster3</t>
   </si>
 </sst>
 </file>
@@ -207,11 +231,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -295,7 +319,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -306,6 +330,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="22.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,7 +356,7 @@
       </c>
     </row>
     <row r="3" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" s="10" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="10" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
@@ -353,33 +378,87 @@
       <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
+      <c r="H4" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="12" t="n">
+        <v>0.0147</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="12" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12"/>
@@ -646,6 +725,9 @@
   <mergeCells count="1">
     <mergeCell ref="H1:J1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" display="https://github.com/NomisCiri/eeg_manypipes_arc/blob/main/REPORT.txt"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>